<commit_message>
Finished adding top 30 WRs since 2007
</commit_message>
<xml_diff>
--- a/data_formatted/formatted_wr.xlsx
+++ b/data_formatted/formatted_wr.xlsx
@@ -21,6 +21,157 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="152">
   <si>
+    <t>Smith, Steve</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>Moore, Lance</t>
+  </si>
+  <si>
+    <t>Johnson, Stevie</t>
+  </si>
+  <si>
+    <t>BUF</t>
+  </si>
+  <si>
+    <t>Shorts, Cecil</t>
+  </si>
+  <si>
+    <t>JAC</t>
+  </si>
+  <si>
+    <t>Smith, Torrey</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Team</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDC</t>
+  </si>
+  <si>
+    <t>Floyd, Malcom</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>Heyward-Bey, Darrius</t>
+  </si>
+  <si>
+    <t>Jackson, DeSean</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>Gaffney, Jabar</t>
+  </si>
+  <si>
+    <t>Lloyd, Brandon</t>
+  </si>
+  <si>
+    <t>Brown, Antonio</t>
+  </si>
+  <si>
+    <t>Garcon, Pierre</t>
+  </si>
+  <si>
+    <t>Johnson, Steve</t>
+  </si>
+  <si>
+    <t>KCC</t>
+  </si>
+  <si>
+    <t>Bowe, Dwayne</t>
+  </si>
+  <si>
+    <t>Jennings, Greg</t>
+  </si>
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>Washington, Nate</t>
+  </si>
+  <si>
+    <t>Robinson, Laurent</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>Nicks, Hakeem</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>Harvin, Percy</t>
+  </si>
+  <si>
+    <t>ARI</t>
+  </si>
+  <si>
+    <t>Fitzgerald, Larry</t>
+  </si>
+  <si>
+    <t>End of 2010 Season</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>Owens, Terrell</t>
+  </si>
+  <si>
+    <t>Manningham, Mario</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Moss, Santana</t>
+  </si>
+  <si>
+    <t>Edwards, Braylon</t>
+  </si>
+  <si>
+    <t>NYJ</t>
+  </si>
+  <si>
+    <t>Johnson, Chad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Britt, Kenny</t>
   </si>
   <si>
@@ -40,9 +191,6 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Ochocinco, Chad</t>
-  </si>
-  <si>
     <t>Holmes, Santonio</t>
   </si>
   <si>
@@ -356,165 +504,12 @@
   </si>
   <si>
     <t>Williams, Mike</t>
-  </si>
-  <si>
-    <t>Smith, Steve</t>
-  </si>
-  <si>
-    <t>CAR</t>
-  </si>
-  <si>
-    <t>Moore, Lance</t>
-  </si>
-  <si>
-    <t>Johnson, Stevie</t>
-  </si>
-  <si>
-    <t>BUF</t>
-  </si>
-  <si>
-    <t>Shorts, Cecil</t>
-  </si>
-  <si>
-    <t>JAC</t>
-  </si>
-  <si>
-    <t>Smith, Torrey</t>
-  </si>
-  <si>
-    <t>BAL</t>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Year</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SDC</t>
-  </si>
-  <si>
-    <t>Floyd, Malcom</t>
-  </si>
-  <si>
-    <t>OAK</t>
-  </si>
-  <si>
-    <t>Heyward-Bey, Darrius</t>
-  </si>
-  <si>
-    <t>Jackson, DeSean</t>
-  </si>
-  <si>
-    <t>WAS</t>
-  </si>
-  <si>
-    <t>Gaffney, Jabar</t>
-  </si>
-  <si>
-    <t>Lloyd, Brandon</t>
-  </si>
-  <si>
-    <t>Brown, Antonio</t>
-  </si>
-  <si>
-    <t>Garcon, Pierre</t>
-  </si>
-  <si>
-    <t>Johnson, Steve</t>
-  </si>
-  <si>
-    <t>KCC</t>
-  </si>
-  <si>
-    <t>Bowe, Dwayne</t>
-  </si>
-  <si>
-    <t>Jennings, Greg</t>
-  </si>
-  <si>
-    <t>TEN</t>
-  </si>
-  <si>
-    <t>Washington, Nate</t>
-  </si>
-  <si>
-    <t>Robinson, Laurent</t>
-  </si>
-  <si>
-    <t>MIA</t>
-  </si>
-  <si>
-    <t>Nicks, Hakeem</t>
-  </si>
-  <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>Harvin, Percy</t>
-  </si>
-  <si>
-    <t>ARI</t>
-  </si>
-  <si>
-    <t>Fitzgerald, Larry</t>
-  </si>
-  <si>
-    <t>End of 2010 Season</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>TB</t>
-  </si>
-  <si>
-    <t>Owens, Terrell</t>
-  </si>
-  <si>
-    <t>Manningham, Mario</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Moss, Santana</t>
-  </si>
-  <si>
-    <t>Edwards, Braylon</t>
-  </si>
-  <si>
-    <t>NYJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -545,8 +540,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:W186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -892,73 +890,73 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" t="s">
+        <v>114</v>
+      </c>
+      <c r="T1" t="s">
         <v>115</v>
       </c>
-      <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="U1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" t="s">
+      <c r="V1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
+      <c r="W1" t="s">
         <v>118</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T1" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -966,16 +964,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C2">
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F2">
         <v>2012</v>
@@ -1013,16 +1011,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C3">
         <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="F3">
         <v>2012</v>
@@ -1063,16 +1061,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="C4">
         <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F4">
         <v>2012</v>
@@ -1116,16 +1114,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="C5">
         <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F5">
         <v>2012</v>
@@ -1169,16 +1167,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C6">
         <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F6">
         <v>2012</v>
@@ -1216,16 +1214,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="C7">
         <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="F7">
         <v>2012</v>
@@ -1260,16 +1258,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="C8">
         <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F8">
         <v>2012</v>
@@ -1304,16 +1302,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="C9">
         <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="F9">
         <v>2012</v>
@@ -1348,16 +1346,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="C10">
         <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F10">
         <v>2012</v>
@@ -1398,16 +1396,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="C11">
         <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F11">
         <v>2012</v>
@@ -1442,16 +1440,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="C12">
         <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="F12">
         <v>2012</v>
@@ -1495,16 +1493,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C13">
         <v>122</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="F13">
         <v>2012</v>
@@ -1542,16 +1540,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="C14">
         <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F14">
         <v>2012</v>
@@ -1586,16 +1584,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="C15">
         <v>124</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="F15">
         <v>2012</v>
@@ -1636,16 +1634,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="C16">
         <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F16">
         <v>2012</v>
@@ -1689,16 +1687,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="C17">
         <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F17">
         <v>2012</v>
@@ -1733,16 +1731,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="C18">
         <v>127</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F18">
         <v>2012</v>
@@ -1786,16 +1784,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="C19">
         <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="F19">
         <v>2012</v>
@@ -1830,16 +1828,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>2012</v>
@@ -1883,16 +1881,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="F21">
         <v>2012</v>
@@ -1927,16 +1925,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>2012</v>
@@ -1974,16 +1972,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>132</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="F23">
         <v>2012</v>
@@ -2027,16 +2025,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>133</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <v>2012</v>
@@ -2077,16 +2075,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C25">
         <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F25">
         <v>2012</v>
@@ -2127,16 +2125,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="C26">
         <v>135</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F26">
         <v>2012</v>
@@ -2180,16 +2178,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="C27">
         <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F27">
         <v>2012</v>
@@ -2227,16 +2225,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>137</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F28">
         <v>2012</v>
@@ -2274,16 +2272,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="C29">
         <v>138</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="F29">
         <v>2012</v>
@@ -2324,16 +2322,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="C30">
         <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="F30">
         <v>2012</v>
@@ -2374,16 +2372,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>140</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F31">
         <v>2012</v>
@@ -2415,73 +2413,73 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I32" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32" t="s">
+        <v>105</v>
+      </c>
+      <c r="K32" t="s">
+        <v>106</v>
+      </c>
+      <c r="L32" t="s">
+        <v>107</v>
+      </c>
+      <c r="M32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N32" t="s">
+        <v>109</v>
+      </c>
+      <c r="O32" t="s">
+        <v>110</v>
+      </c>
+      <c r="P32" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>112</v>
+      </c>
+      <c r="R32" t="s">
+        <v>113</v>
+      </c>
+      <c r="S32" t="s">
+        <v>114</v>
+      </c>
+      <c r="T32" t="s">
         <v>115</v>
       </c>
-      <c r="C32" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="U32" t="s">
         <v>116</v>
       </c>
-      <c r="E32" t="s">
+      <c r="V32" t="s">
         <v>117</v>
       </c>
-      <c r="F32" t="s">
+      <c r="W32" t="s">
         <v>118</v>
-      </c>
-      <c r="G32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" t="s">
-        <v>55</v>
-      </c>
-      <c r="I32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32" t="s">
-        <v>59</v>
-      </c>
-      <c r="L32" t="s">
-        <v>60</v>
-      </c>
-      <c r="M32" t="s">
-        <v>61</v>
-      </c>
-      <c r="N32" t="s">
-        <v>62</v>
-      </c>
-      <c r="O32" t="s">
-        <v>63</v>
-      </c>
-      <c r="P32" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>65</v>
-      </c>
-      <c r="R32" t="s">
-        <v>66</v>
-      </c>
-      <c r="S32" t="s">
-        <v>67</v>
-      </c>
-      <c r="T32" t="s">
-        <v>68</v>
-      </c>
-      <c r="U32" t="s">
-        <v>69</v>
-      </c>
-      <c r="V32" t="s">
-        <v>70</v>
-      </c>
-      <c r="W32" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -2489,16 +2487,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C33">
         <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F33">
         <v>2011</v>
@@ -2542,16 +2540,16 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>140</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F34">
         <v>2011</v>
@@ -2586,16 +2584,16 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="C35">
         <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="F35">
         <v>2011</v>
@@ -2636,16 +2634,16 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="C36">
         <v>123</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F36">
         <v>2011</v>
@@ -2689,16 +2687,16 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F37">
         <v>2011</v>
@@ -2733,16 +2731,16 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="F38">
         <v>2011</v>
@@ -2786,16 +2784,16 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="C39">
         <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F39">
         <v>2011</v>
@@ -2830,16 +2828,16 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
       <c r="C40">
         <v>142</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="F40">
         <v>2011</v>
@@ -2886,16 +2884,16 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="C41">
         <v>135</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F41">
         <v>2011</v>
@@ -2939,16 +2937,16 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="C42">
         <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E42" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="F42">
         <v>2011</v>
@@ -2989,16 +2987,16 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="C43">
         <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F43">
         <v>2011</v>
@@ -3033,16 +3031,16 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C44">
         <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="F44">
         <v>2011</v>
@@ -3080,16 +3078,16 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C45">
         <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="F45">
         <v>2011</v>
@@ -3133,16 +3131,16 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="C46">
         <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F46">
         <v>2011</v>
@@ -3183,16 +3181,16 @@
         <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="C47">
         <v>144</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F47">
         <v>2011</v>
@@ -3227,16 +3225,16 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="C48">
         <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="F48">
         <v>2011</v>
@@ -3280,16 +3278,16 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C49">
         <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E49" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F49">
         <v>2011</v>
@@ -3324,16 +3322,16 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="C50">
         <v>119</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F50">
         <v>2011</v>
@@ -3377,16 +3375,16 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="C51">
         <v>147</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E51" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="F51">
         <v>2011</v>
@@ -3427,16 +3425,16 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="C52">
         <v>113</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F52">
         <v>2011</v>
@@ -3480,16 +3478,16 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
       <c r="C53">
         <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F53">
         <v>2011</v>
@@ -3524,16 +3522,16 @@
         <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="C54">
         <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E54" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F54">
         <v>2011</v>
@@ -3574,16 +3572,16 @@
         <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="C55">
         <v>148</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F55">
         <v>2011</v>
@@ -3627,16 +3625,16 @@
         <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="C56">
         <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E56" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F56">
         <v>2011</v>
@@ -3677,16 +3675,16 @@
         <v>25</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="C57">
         <v>150</v>
       </c>
       <c r="D57" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E57" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F57">
         <v>2011</v>
@@ -3721,16 +3719,16 @@
         <v>26</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <v>151</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E58" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="F58">
         <v>2011</v>
@@ -3768,16 +3766,16 @@
         <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="C59">
         <v>152</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E59" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F59">
         <v>2011</v>
@@ -3821,16 +3819,16 @@
         <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="C60">
         <v>125</v>
       </c>
       <c r="D60" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E60" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F60">
         <v>2011</v>
@@ -3865,16 +3863,16 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="C61">
         <v>153</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E61" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="F61">
         <v>2011</v>
@@ -3912,16 +3910,16 @@
         <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="C62">
         <v>154</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E62" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="F62">
         <v>2011</v>
@@ -3953,73 +3951,73 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" t="s">
+        <v>101</v>
+      </c>
+      <c r="H63" t="s">
+        <v>102</v>
+      </c>
+      <c r="I63" t="s">
+        <v>104</v>
+      </c>
+      <c r="J63" t="s">
+        <v>105</v>
+      </c>
+      <c r="K63" t="s">
+        <v>106</v>
+      </c>
+      <c r="L63" t="s">
+        <v>107</v>
+      </c>
+      <c r="M63" t="s">
+        <v>108</v>
+      </c>
+      <c r="N63" t="s">
+        <v>109</v>
+      </c>
+      <c r="O63" t="s">
+        <v>110</v>
+      </c>
+      <c r="P63" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>112</v>
+      </c>
+      <c r="R63" t="s">
+        <v>113</v>
+      </c>
+      <c r="S63" t="s">
+        <v>114</v>
+      </c>
+      <c r="T63" t="s">
         <v>115</v>
       </c>
-      <c r="C63" t="s">
-        <v>114</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="U63" t="s">
         <v>116</v>
       </c>
-      <c r="E63" t="s">
+      <c r="V63" t="s">
         <v>117</v>
       </c>
-      <c r="F63" t="s">
+      <c r="W63" t="s">
         <v>118</v>
-      </c>
-      <c r="G63" t="s">
-        <v>54</v>
-      </c>
-      <c r="H63" t="s">
-        <v>55</v>
-      </c>
-      <c r="I63" t="s">
-        <v>57</v>
-      </c>
-      <c r="J63" t="s">
-        <v>58</v>
-      </c>
-      <c r="K63" t="s">
-        <v>59</v>
-      </c>
-      <c r="L63" t="s">
-        <v>60</v>
-      </c>
-      <c r="M63" t="s">
-        <v>61</v>
-      </c>
-      <c r="N63" t="s">
-        <v>62</v>
-      </c>
-      <c r="O63" t="s">
-        <v>63</v>
-      </c>
-      <c r="P63" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>65</v>
-      </c>
-      <c r="R63" t="s">
-        <v>66</v>
-      </c>
-      <c r="S63" t="s">
-        <v>67</v>
-      </c>
-      <c r="T63" t="s">
-        <v>68</v>
-      </c>
-      <c r="U63" t="s">
-        <v>69</v>
-      </c>
-      <c r="V63" t="s">
-        <v>70</v>
-      </c>
-      <c r="W63" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:23">
@@ -4027,13 +4025,16 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>21</v>
+      </c>
+      <c r="C64">
+        <v>150</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E64" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F64">
         <v>2010</v>
@@ -4074,13 +4075,16 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>26</v>
+      </c>
+      <c r="C65">
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E65" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="F65">
         <v>2010</v>
@@ -4121,13 +4125,16 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C66">
+        <v>146</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F66">
         <v>2010</v>
@@ -4168,13 +4175,16 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="C67">
+        <v>120</v>
       </c>
       <c r="D67" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E67" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F67">
         <v>2010</v>
@@ -4218,13 +4228,16 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>45</v>
+        <v>92</v>
+      </c>
+      <c r="C68">
+        <v>135</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E68" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F68">
         <v>2010</v>
@@ -4265,13 +4278,16 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>119</v>
+      </c>
+      <c r="C69">
+        <v>111</v>
       </c>
       <c r="D69" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E69" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F69">
         <v>2010</v>
@@ -4312,13 +4328,16 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>32</v>
+      </c>
+      <c r="C70">
+        <v>143</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E70" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F70">
         <v>2010</v>
@@ -4353,13 +4372,16 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>133</v>
+      </c>
+      <c r="C71" s="1">
+        <v>118</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E71" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="F71">
         <v>2010</v>
@@ -4400,13 +4422,16 @@
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>146</v>
+      </c>
+      <c r="C72">
+        <v>125</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E72" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F72">
         <v>2010</v>
@@ -4444,13 +4469,16 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <v>131</v>
       </c>
       <c r="D73" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E73" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F73">
         <v>2010</v>
@@ -4488,13 +4516,16 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>47</v>
+        <v>94</v>
+      </c>
+      <c r="C74">
+        <v>136</v>
       </c>
       <c r="D74" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E74" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F74">
         <v>2010</v>
@@ -4541,13 +4572,16 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>104</v>
+        <v>151</v>
+      </c>
+      <c r="C75">
+        <v>128</v>
       </c>
       <c r="D75" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E75" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="F75">
         <v>2010</v>
@@ -4585,13 +4619,16 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>48</v>
+        <v>95</v>
+      </c>
+      <c r="C76">
+        <v>137</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E76" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F76">
         <v>2010</v>
@@ -4635,13 +4672,16 @@
         <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>123</v>
+        <v>18</v>
+      </c>
+      <c r="C77">
+        <v>152</v>
       </c>
       <c r="D77" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E77" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F77">
         <v>2010</v>
@@ -4688,13 +4728,16 @@
         <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="C78">
+        <v>155</v>
       </c>
       <c r="D78" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E78" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F78">
         <v>2010</v>
@@ -4729,13 +4772,16 @@
         <v>16</v>
       </c>
       <c r="B79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79">
         <v>141</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E79" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F79">
         <v>2010</v>
@@ -4770,13 +4816,16 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>42</v>
+      </c>
+      <c r="C80">
+        <v>156</v>
       </c>
       <c r="D80" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E80" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F80">
         <v>2010</v>
@@ -4820,13 +4869,16 @@
         <v>18</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>140</v>
+      </c>
+      <c r="C81">
+        <v>122</v>
       </c>
       <c r="D81" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E81" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="F81">
         <v>2010</v>
@@ -4867,13 +4919,16 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>149</v>
+        <v>44</v>
+      </c>
+      <c r="C82">
+        <v>157</v>
       </c>
       <c r="D82" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E82" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="F82">
         <v>2010</v>
@@ -4917,13 +4972,16 @@
         <v>20</v>
       </c>
       <c r="B83" t="s">
-        <v>139</v>
+        <v>34</v>
+      </c>
+      <c r="C83">
+        <v>142</v>
       </c>
       <c r="D83" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E83" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="F83">
         <v>2010</v>
@@ -4967,13 +5025,16 @@
         <v>21</v>
       </c>
       <c r="B84" t="s">
-        <v>150</v>
+        <v>45</v>
+      </c>
+      <c r="C84">
+        <v>158</v>
       </c>
       <c r="D84" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E84" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="F84">
         <v>2010</v>
@@ -5017,13 +5078,16 @@
         <v>22</v>
       </c>
       <c r="B85" t="s">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="C85">
+        <v>159</v>
       </c>
       <c r="D85" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E85" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="F85">
         <v>2010</v>
@@ -5061,13 +5125,16 @@
         <v>23</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>138</v>
+      </c>
+      <c r="C86">
+        <v>121</v>
       </c>
       <c r="D86" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E86" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F86">
         <v>2010</v>
@@ -5102,13 +5169,16 @@
         <v>24</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="C87">
+        <v>160</v>
       </c>
       <c r="D87" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E87" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="F87">
         <v>2010</v>
@@ -5152,13 +5222,16 @@
         <v>25</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="C88">
+        <v>161</v>
       </c>
       <c r="D88" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E88" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F88">
         <v>2010</v>
@@ -5202,13 +5275,16 @@
         <v>26</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>2</v>
+      </c>
+      <c r="C89">
+        <v>130</v>
       </c>
       <c r="D89" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E89" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="F89">
         <v>2010</v>
@@ -5246,13 +5322,16 @@
         <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="C90">
+        <v>162</v>
       </c>
       <c r="D90" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E90" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F90">
         <v>2010</v>
@@ -5287,13 +5366,16 @@
         <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>122</v>
+      </c>
+      <c r="C91">
+        <v>112</v>
       </c>
       <c r="D91" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E91" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="F91">
         <v>2010</v>
@@ -5337,13 +5419,16 @@
         <v>29</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>88</v>
+      </c>
+      <c r="C92">
+        <v>163</v>
       </c>
       <c r="D92" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E92" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="F92">
         <v>2010</v>
@@ -5384,13 +5469,16 @@
         <v>30</v>
       </c>
       <c r="B93" t="s">
-        <v>42</v>
+        <v>89</v>
+      </c>
+      <c r="C93">
+        <v>164</v>
       </c>
       <c r="D93" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E93" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="F93">
         <v>2010</v>
@@ -5425,73 +5513,73 @@
     </row>
     <row r="94" spans="1:23">
       <c r="A94" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" t="s">
+        <v>101</v>
+      </c>
+      <c r="H94" t="s">
+        <v>102</v>
+      </c>
+      <c r="I94" t="s">
+        <v>104</v>
+      </c>
+      <c r="J94" t="s">
+        <v>105</v>
+      </c>
+      <c r="K94" t="s">
+        <v>106</v>
+      </c>
+      <c r="L94" t="s">
+        <v>107</v>
+      </c>
+      <c r="M94" t="s">
+        <v>108</v>
+      </c>
+      <c r="N94" t="s">
+        <v>109</v>
+      </c>
+      <c r="O94" t="s">
+        <v>110</v>
+      </c>
+      <c r="P94" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>112</v>
+      </c>
+      <c r="R94" t="s">
+        <v>113</v>
+      </c>
+      <c r="S94" t="s">
+        <v>114</v>
+      </c>
+      <c r="T94" t="s">
         <v>115</v>
       </c>
-      <c r="C94" t="s">
-        <v>114</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="U94" t="s">
         <v>116</v>
       </c>
-      <c r="E94" t="s">
+      <c r="V94" t="s">
         <v>117</v>
       </c>
-      <c r="F94" t="s">
+      <c r="W94" t="s">
         <v>118</v>
-      </c>
-      <c r="G94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H94" t="s">
-        <v>55</v>
-      </c>
-      <c r="I94" t="s">
-        <v>57</v>
-      </c>
-      <c r="J94" t="s">
-        <v>58</v>
-      </c>
-      <c r="K94" t="s">
-        <v>59</v>
-      </c>
-      <c r="L94" t="s">
-        <v>60</v>
-      </c>
-      <c r="M94" t="s">
-        <v>61</v>
-      </c>
-      <c r="N94" t="s">
-        <v>62</v>
-      </c>
-      <c r="O94" t="s">
-        <v>63</v>
-      </c>
-      <c r="P94" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>65</v>
-      </c>
-      <c r="R94" t="s">
-        <v>66</v>
-      </c>
-      <c r="S94" t="s">
-        <v>67</v>
-      </c>
-      <c r="T94" t="s">
-        <v>68</v>
-      </c>
-      <c r="U94" t="s">
-        <v>69</v>
-      </c>
-      <c r="V94" t="s">
-        <v>70</v>
-      </c>
-      <c r="W94" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:23">
@@ -5499,13 +5587,16 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>86</v>
+        <v>133</v>
+      </c>
+      <c r="C95">
+        <v>118</v>
       </c>
       <c r="D95" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E95" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="F95">
         <v>2009</v>
@@ -5546,13 +5637,16 @@
         <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>52</v>
+      </c>
+      <c r="C96">
+        <v>165</v>
       </c>
       <c r="D96" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E96" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F96">
         <v>2009</v>
@@ -5596,13 +5690,16 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>47</v>
+        <v>94</v>
+      </c>
+      <c r="C97">
+        <v>136</v>
       </c>
       <c r="D97" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E97" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F97">
         <v>2009</v>
@@ -5643,13 +5740,16 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>123</v>
+        <v>18</v>
+      </c>
+      <c r="C98">
+        <v>152</v>
       </c>
       <c r="D98" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E98" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F98">
         <v>2009</v>
@@ -5696,13 +5796,16 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99">
         <v>141</v>
       </c>
       <c r="D99" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E99" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F99">
         <v>2009</v>
@@ -5743,13 +5846,16 @@
         <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>146</v>
+      </c>
+      <c r="C100">
+        <v>125</v>
       </c>
       <c r="D100" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E100" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F100">
         <v>2009</v>
@@ -5793,13 +5899,16 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="C101">
+        <v>120</v>
       </c>
       <c r="D101" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E101" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F101">
         <v>2009</v>
@@ -5840,13 +5949,16 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>51</v>
+        <v>98</v>
+      </c>
+      <c r="C102">
+        <v>139</v>
       </c>
       <c r="D102" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E102" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="F102">
         <v>2009</v>
@@ -5890,13 +6002,16 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>75</v>
+        <v>122</v>
+      </c>
+      <c r="C103">
+        <v>112</v>
       </c>
       <c r="D103" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E103" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F103">
         <v>2009</v>
@@ -5937,13 +6052,16 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>83</v>
+        <v>130</v>
+      </c>
+      <c r="C104">
+        <v>116</v>
       </c>
       <c r="D104" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E104" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="F104">
         <v>2009</v>
@@ -5984,13 +6102,16 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E105" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F105">
         <v>2009</v>
@@ -6031,13 +6152,16 @@
         <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>138</v>
+      </c>
+      <c r="C106">
+        <v>121</v>
       </c>
       <c r="D106" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E106" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F106">
         <v>2009</v>
@@ -6078,13 +6202,16 @@
         <v>13</v>
       </c>
       <c r="B107" t="s">
-        <v>93</v>
+        <v>140</v>
+      </c>
+      <c r="C107">
+        <v>122</v>
       </c>
       <c r="D107" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E107" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="F107">
         <v>2009</v>
@@ -6128,13 +6255,16 @@
         <v>14</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="C108">
+        <v>167</v>
       </c>
       <c r="D108" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E108" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F108">
         <v>2009</v>
@@ -6178,13 +6308,16 @@
         <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>54</v>
+      </c>
+      <c r="C109">
+        <v>168</v>
       </c>
       <c r="D109" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E109" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F109">
         <v>2009</v>
@@ -6228,13 +6361,16 @@
         <v>16</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="C110">
+        <v>169</v>
       </c>
       <c r="D110" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E110" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F110">
         <v>2009</v>
@@ -6278,13 +6414,16 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="C111">
+        <v>162</v>
       </c>
       <c r="D111" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E111" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F111">
         <v>2009</v>
@@ -6325,13 +6464,16 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>129</v>
       </c>
       <c r="D112" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E112" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="F112">
         <v>2009</v>
@@ -6372,13 +6514,16 @@
         <v>19</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="C113">
+        <v>170</v>
       </c>
       <c r="D113" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E113" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F113">
         <v>2009</v>
@@ -6422,13 +6567,16 @@
         <v>20</v>
       </c>
       <c r="B114" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C114">
+        <v>146</v>
       </c>
       <c r="D114" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E114" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F114">
         <v>2009</v>
@@ -6469,13 +6617,16 @@
         <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="C115">
+        <v>171</v>
       </c>
       <c r="D115" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E115" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="F115">
         <v>2009</v>
@@ -6519,13 +6670,16 @@
         <v>22</v>
       </c>
       <c r="B116" t="s">
-        <v>72</v>
+        <v>119</v>
+      </c>
+      <c r="C116">
+        <v>111</v>
       </c>
       <c r="D116" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E116" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F116">
         <v>2009</v>
@@ -6569,13 +6723,16 @@
         <v>23</v>
       </c>
       <c r="B117" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="C117">
+        <v>161</v>
       </c>
       <c r="D117" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E117" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F117">
         <v>2009</v>
@@ -6622,13 +6779,16 @@
         <v>24</v>
       </c>
       <c r="B118" t="s">
-        <v>139</v>
+        <v>34</v>
+      </c>
+      <c r="C118">
+        <v>142</v>
       </c>
       <c r="D118" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E118" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="F118">
         <v>2009</v>
@@ -6669,13 +6829,16 @@
         <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="C119">
+        <v>172</v>
       </c>
       <c r="D119" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E119" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="F119">
         <v>2009</v>
@@ -6719,13 +6882,16 @@
         <v>26</v>
       </c>
       <c r="B120" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="C120">
+        <v>155</v>
       </c>
       <c r="D120" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E120" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F120">
         <v>2009</v>
@@ -6769,13 +6935,16 @@
         <v>27</v>
       </c>
       <c r="B121" t="s">
-        <v>137</v>
+        <v>32</v>
+      </c>
+      <c r="C121">
+        <v>143</v>
       </c>
       <c r="D121" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E121" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F121">
         <v>2009</v>
@@ -6816,13 +6985,16 @@
         <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>45</v>
+        <v>92</v>
+      </c>
+      <c r="C122">
+        <v>135</v>
       </c>
       <c r="D122" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E122" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F122">
         <v>2009</v>
@@ -6866,13 +7038,16 @@
         <v>29</v>
       </c>
       <c r="B123" t="s">
-        <v>147</v>
+        <v>42</v>
+      </c>
+      <c r="C123">
+        <v>156</v>
       </c>
       <c r="D123" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E123" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F123">
         <v>2009</v>
@@ -6916,13 +7091,13 @@
         <v>30</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="D124" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E124" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F124">
         <v>2009</v>
@@ -6960,73 +7135,73 @@
     </row>
     <row r="125" spans="1:23">
       <c r="A125" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="B125" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" t="s">
+        <v>11</v>
+      </c>
+      <c r="E125" t="s">
+        <v>12</v>
+      </c>
+      <c r="F125" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125" t="s">
+        <v>101</v>
+      </c>
+      <c r="H125" t="s">
+        <v>102</v>
+      </c>
+      <c r="I125" t="s">
+        <v>104</v>
+      </c>
+      <c r="J125" t="s">
+        <v>105</v>
+      </c>
+      <c r="K125" t="s">
+        <v>106</v>
+      </c>
+      <c r="L125" t="s">
+        <v>107</v>
+      </c>
+      <c r="M125" t="s">
+        <v>108</v>
+      </c>
+      <c r="N125" t="s">
+        <v>109</v>
+      </c>
+      <c r="O125" t="s">
+        <v>110</v>
+      </c>
+      <c r="P125" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>112</v>
+      </c>
+      <c r="R125" t="s">
+        <v>113</v>
+      </c>
+      <c r="S125" t="s">
+        <v>114</v>
+      </c>
+      <c r="T125" t="s">
         <v>115</v>
       </c>
-      <c r="C125" t="s">
-        <v>114</v>
-      </c>
-      <c r="D125" t="s">
+      <c r="U125" t="s">
         <v>116</v>
       </c>
-      <c r="E125" t="s">
+      <c r="V125" t="s">
         <v>117</v>
       </c>
-      <c r="F125" t="s">
+      <c r="W125" t="s">
         <v>118</v>
-      </c>
-      <c r="G125" t="s">
-        <v>54</v>
-      </c>
-      <c r="H125" t="s">
-        <v>55</v>
-      </c>
-      <c r="I125" t="s">
-        <v>57</v>
-      </c>
-      <c r="J125" t="s">
-        <v>58</v>
-      </c>
-      <c r="K125" t="s">
-        <v>59</v>
-      </c>
-      <c r="L125" t="s">
-        <v>60</v>
-      </c>
-      <c r="M125" t="s">
-        <v>61</v>
-      </c>
-      <c r="N125" t="s">
-        <v>62</v>
-      </c>
-      <c r="O125" t="s">
-        <v>63</v>
-      </c>
-      <c r="P125" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q125" t="s">
-        <v>65</v>
-      </c>
-      <c r="R125" t="s">
-        <v>66</v>
-      </c>
-      <c r="S125" t="s">
-        <v>67</v>
-      </c>
-      <c r="T125" t="s">
-        <v>68</v>
-      </c>
-      <c r="U125" t="s">
-        <v>69</v>
-      </c>
-      <c r="V125" t="s">
-        <v>70</v>
-      </c>
-      <c r="W125" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="126" spans="1:23">
@@ -7034,13 +7209,16 @@
         <v>1</v>
       </c>
       <c r="B126" t="s">
+        <v>36</v>
+      </c>
+      <c r="C126">
         <v>141</v>
       </c>
       <c r="D126" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E126" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F126">
         <v>2008</v>
@@ -7090,13 +7268,16 @@
         <v>2</v>
       </c>
       <c r="B127" t="s">
-        <v>86</v>
+        <v>133</v>
+      </c>
+      <c r="C127">
+        <v>118</v>
       </c>
       <c r="D127" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E127" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="F127">
         <v>2008</v>
@@ -7146,13 +7327,16 @@
         <v>3</v>
       </c>
       <c r="B128" t="s">
-        <v>72</v>
+        <v>119</v>
+      </c>
+      <c r="C128">
+        <v>111</v>
       </c>
       <c r="D128" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E128" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F128">
         <v>2008</v>
@@ -7202,13 +7386,16 @@
         <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C129">
+        <v>146</v>
       </c>
       <c r="D129" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E129" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F129">
         <v>2008</v>
@@ -7258,13 +7445,16 @@
         <v>5</v>
       </c>
       <c r="B130" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>129</v>
       </c>
       <c r="D130" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E130" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="F130">
         <v>2008</v>
@@ -7314,13 +7504,16 @@
         <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="C131">
+        <v>120</v>
       </c>
       <c r="D131" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E131" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F131">
         <v>2008</v>
@@ -7370,13 +7563,16 @@
         <v>7</v>
       </c>
       <c r="B132" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="C132">
+        <v>161</v>
       </c>
       <c r="D132" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E132" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F132">
         <v>2008</v>
@@ -7426,13 +7622,16 @@
         <v>8</v>
       </c>
       <c r="B133" t="s">
-        <v>23</v>
+        <v>70</v>
+      </c>
+      <c r="C133">
+        <v>173</v>
       </c>
       <c r="D133" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E133" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="F133">
         <v>2008</v>
@@ -7482,13 +7681,16 @@
         <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="C134">
+        <v>155</v>
       </c>
       <c r="D134" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E134" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F134">
         <v>2008</v>
@@ -7538,13 +7740,16 @@
         <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>52</v>
+      </c>
+      <c r="C135">
+        <v>165</v>
       </c>
       <c r="D135" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E135" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F135">
         <v>2008</v>
@@ -7594,13 +7799,16 @@
         <v>11</v>
       </c>
       <c r="B136" t="s">
-        <v>83</v>
+        <v>130</v>
+      </c>
+      <c r="C136">
+        <v>116</v>
       </c>
       <c r="D136" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E136" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="F136">
         <v>2008</v>
@@ -7650,13 +7858,16 @@
         <v>12</v>
       </c>
       <c r="B137" t="s">
-        <v>75</v>
+        <v>122</v>
+      </c>
+      <c r="C137">
+        <v>112</v>
       </c>
       <c r="D137" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E137" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F137">
         <v>2008</v>
@@ -7706,13 +7917,16 @@
         <v>13</v>
       </c>
       <c r="B138" t="s">
-        <v>107</v>
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <v>130</v>
       </c>
       <c r="D138" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E138" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="F138">
         <v>2008</v>
@@ -7762,13 +7976,16 @@
         <v>14</v>
       </c>
       <c r="B139" t="s">
-        <v>99</v>
+        <v>146</v>
+      </c>
+      <c r="C139">
+        <v>125</v>
       </c>
       <c r="D139" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E139" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F139">
         <v>2008</v>
@@ -7818,13 +8035,16 @@
         <v>15</v>
       </c>
       <c r="B140" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="C140">
+        <v>169</v>
       </c>
       <c r="D140" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E140" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F140">
         <v>2008</v>
@@ -7874,13 +8094,16 @@
         <v>16</v>
       </c>
       <c r="B141" t="s">
-        <v>131</v>
+        <v>26</v>
+      </c>
+      <c r="C141">
+        <v>147</v>
       </c>
       <c r="D141" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E141" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="F141">
         <v>2008</v>
@@ -7930,13 +8153,16 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>149</v>
+        <v>44</v>
+      </c>
+      <c r="C142">
+        <v>157</v>
       </c>
       <c r="D142" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E142" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="F142">
         <v>2008</v>
@@ -7986,13 +8212,16 @@
         <v>18</v>
       </c>
       <c r="B143" t="s">
-        <v>21</v>
+        <v>68</v>
+      </c>
+      <c r="C143">
+        <v>174</v>
       </c>
       <c r="D143" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E143" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="F143">
         <v>2008</v>
@@ -8042,13 +8271,16 @@
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>24</v>
+        <v>71</v>
+      </c>
+      <c r="C144">
+        <v>175</v>
       </c>
       <c r="D144" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E144" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="F144">
         <v>2008</v>
@@ -8098,13 +8330,16 @@
         <v>20</v>
       </c>
       <c r="B145" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="C145">
+        <v>176</v>
       </c>
       <c r="D145" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E145" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F145">
         <v>2008</v>
@@ -8154,13 +8389,16 @@
         <v>21</v>
       </c>
       <c r="B146" t="s">
-        <v>91</v>
+        <v>138</v>
+      </c>
+      <c r="C146">
+        <v>121</v>
       </c>
       <c r="D146" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E146" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F146">
         <v>2008</v>
@@ -8210,13 +8448,16 @@
         <v>22</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="C147">
+        <v>162</v>
       </c>
       <c r="D147" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E147" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F147">
         <v>2008</v>
@@ -8266,13 +8507,16 @@
         <v>23</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="C148">
+        <v>170</v>
       </c>
       <c r="D148" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E148" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F148">
         <v>2008</v>
@@ -8322,13 +8566,16 @@
         <v>24</v>
       </c>
       <c r="B149" t="s">
-        <v>26</v>
+        <v>73</v>
+      </c>
+      <c r="C149">
+        <v>177</v>
       </c>
       <c r="D149" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E149" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="F149">
         <v>2008</v>
@@ -8378,13 +8625,16 @@
         <v>25</v>
       </c>
       <c r="B150" t="s">
-        <v>27</v>
+        <v>74</v>
+      </c>
+      <c r="C150">
+        <v>178</v>
       </c>
       <c r="D150" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E150" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="F150">
         <v>2008</v>
@@ -8434,13 +8684,16 @@
         <v>26</v>
       </c>
       <c r="B151" t="s">
-        <v>29</v>
+        <v>76</v>
+      </c>
+      <c r="C151">
+        <v>179</v>
       </c>
       <c r="D151" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E151" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="F151">
         <v>2008</v>
@@ -8490,13 +8743,16 @@
         <v>27</v>
       </c>
       <c r="B152" t="s">
-        <v>15</v>
+        <v>62</v>
+      </c>
+      <c r="C152">
+        <v>180</v>
       </c>
       <c r="D152" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E152" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F152">
         <v>2008</v>
@@ -8546,13 +8802,16 @@
         <v>28</v>
       </c>
       <c r="B153" t="s">
-        <v>18</v>
+        <v>65</v>
+      </c>
+      <c r="C153">
+        <v>181</v>
       </c>
       <c r="D153" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E153" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F153">
         <v>2008</v>
@@ -8602,13 +8861,16 @@
         <v>29</v>
       </c>
       <c r="B154" t="s">
-        <v>123</v>
+        <v>18</v>
+      </c>
+      <c r="C154">
+        <v>152</v>
       </c>
       <c r="D154" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E154" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F154">
         <v>2008</v>
@@ -8658,13 +8920,16 @@
         <v>30</v>
       </c>
       <c r="B155" t="s">
-        <v>13</v>
+        <v>60</v>
+      </c>
+      <c r="C155">
+        <v>182</v>
       </c>
       <c r="D155" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E155" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F155">
         <v>2008</v>
@@ -8711,73 +8976,73 @@
     </row>
     <row r="156" spans="1:23">
       <c r="A156" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" t="s">
+        <v>9</v>
+      </c>
+      <c r="D156" t="s">
+        <v>11</v>
+      </c>
+      <c r="E156" t="s">
+        <v>12</v>
+      </c>
+      <c r="F156" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" t="s">
+        <v>101</v>
+      </c>
+      <c r="H156" t="s">
+        <v>102</v>
+      </c>
+      <c r="I156" t="s">
+        <v>104</v>
+      </c>
+      <c r="J156" t="s">
+        <v>105</v>
+      </c>
+      <c r="K156" t="s">
+        <v>106</v>
+      </c>
+      <c r="L156" t="s">
+        <v>107</v>
+      </c>
+      <c r="M156" t="s">
+        <v>108</v>
+      </c>
+      <c r="N156" t="s">
+        <v>109</v>
+      </c>
+      <c r="O156" t="s">
+        <v>110</v>
+      </c>
+      <c r="P156" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>112</v>
+      </c>
+      <c r="R156" t="s">
+        <v>113</v>
+      </c>
+      <c r="S156" t="s">
+        <v>114</v>
+      </c>
+      <c r="T156" t="s">
         <v>115</v>
       </c>
-      <c r="C156" t="s">
-        <v>114</v>
-      </c>
-      <c r="D156" t="s">
+      <c r="U156" t="s">
         <v>116</v>
       </c>
-      <c r="E156" t="s">
+      <c r="V156" t="s">
         <v>117</v>
       </c>
-      <c r="F156" t="s">
+      <c r="W156" t="s">
         <v>118</v>
-      </c>
-      <c r="G156" t="s">
-        <v>54</v>
-      </c>
-      <c r="H156" t="s">
-        <v>55</v>
-      </c>
-      <c r="I156" t="s">
-        <v>57</v>
-      </c>
-      <c r="J156" t="s">
-        <v>58</v>
-      </c>
-      <c r="K156" t="s">
-        <v>59</v>
-      </c>
-      <c r="L156" t="s">
-        <v>60</v>
-      </c>
-      <c r="M156" t="s">
-        <v>61</v>
-      </c>
-      <c r="N156" t="s">
-        <v>62</v>
-      </c>
-      <c r="O156" t="s">
-        <v>63</v>
-      </c>
-      <c r="P156" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q156" t="s">
-        <v>65</v>
-      </c>
-      <c r="R156" t="s">
-        <v>66</v>
-      </c>
-      <c r="S156" t="s">
-        <v>67</v>
-      </c>
-      <c r="T156" t="s">
-        <v>68</v>
-      </c>
-      <c r="U156" t="s">
-        <v>69</v>
-      </c>
-      <c r="V156" t="s">
-        <v>70</v>
-      </c>
-      <c r="W156" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="157" spans="1:23">
@@ -8785,13 +9050,16 @@
         <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>52</v>
+      </c>
+      <c r="C157">
+        <v>165</v>
       </c>
       <c r="D157" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E157" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F157">
         <v>2007</v>
@@ -8826,13 +9094,16 @@
         <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="C158">
+        <v>155</v>
       </c>
       <c r="D158" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E158" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F158">
         <v>2007</v>
@@ -8873,13 +9144,16 @@
         <v>3</v>
       </c>
       <c r="B159" t="s">
-        <v>150</v>
+        <v>45</v>
+      </c>
+      <c r="C159">
+        <v>158</v>
       </c>
       <c r="D159" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E159" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F159">
         <v>2007</v>
@@ -8917,13 +9191,16 @@
         <v>4</v>
       </c>
       <c r="B160" t="s">
-        <v>99</v>
+        <v>146</v>
+      </c>
+      <c r="C160">
+        <v>125</v>
       </c>
       <c r="D160" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E160" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F160">
         <v>2007</v>
@@ -8967,13 +9244,16 @@
         <v>5</v>
       </c>
       <c r="B161" t="s">
+        <v>36</v>
+      </c>
+      <c r="C161">
         <v>141</v>
       </c>
       <c r="D161" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E161" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F161">
         <v>2007</v>
@@ -9011,13 +9291,16 @@
         <v>6</v>
       </c>
       <c r="B162" t="s">
-        <v>33</v>
+        <v>80</v>
+      </c>
+      <c r="C162">
+        <v>167</v>
       </c>
       <c r="D162" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E162" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F162">
         <v>2007</v>
@@ -9061,13 +9344,16 @@
         <v>7</v>
       </c>
       <c r="B163" t="s">
-        <v>13</v>
+        <v>60</v>
+      </c>
+      <c r="C163">
+        <v>182</v>
       </c>
       <c r="D163" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E163" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="F163">
         <v>2007</v>
@@ -9111,13 +9397,16 @@
         <v>8</v>
       </c>
       <c r="B164" t="s">
-        <v>93</v>
+        <v>140</v>
+      </c>
+      <c r="C164">
+        <v>122</v>
       </c>
       <c r="D164" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E164" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="F164">
         <v>2007</v>
@@ -9155,13 +9444,16 @@
         <v>9</v>
       </c>
       <c r="B165" t="s">
-        <v>75</v>
+        <v>122</v>
+      </c>
+      <c r="C165">
+        <v>112</v>
       </c>
       <c r="D165" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E165" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F165">
         <v>2007</v>
@@ -9205,13 +9497,16 @@
         <v>10</v>
       </c>
       <c r="B166" t="s">
-        <v>31</v>
+        <v>78</v>
+      </c>
+      <c r="C166">
+        <v>183</v>
       </c>
       <c r="D166" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E166" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F166">
         <v>2007</v>
@@ -9246,13 +9541,16 @@
         <v>11</v>
       </c>
       <c r="B167" t="s">
-        <v>91</v>
+        <v>138</v>
+      </c>
+      <c r="C167">
+        <v>121</v>
       </c>
       <c r="D167" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E167" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F167">
         <v>2007</v>
@@ -9293,13 +9591,16 @@
         <v>12</v>
       </c>
       <c r="B168" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C168">
+        <v>146</v>
       </c>
       <c r="D168" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E168" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F168">
         <v>2007</v>
@@ -9334,13 +9635,16 @@
         <v>13</v>
       </c>
       <c r="B169" t="s">
-        <v>30</v>
+        <v>77</v>
+      </c>
+      <c r="C169">
+        <v>184</v>
       </c>
       <c r="D169" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E169" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="F169">
         <v>2007</v>
@@ -9378,13 +9682,16 @@
         <v>14</v>
       </c>
       <c r="B170" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="C170">
+        <v>120</v>
       </c>
       <c r="D170" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E170" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F170">
         <v>2007</v>
@@ -9425,13 +9732,16 @@
         <v>15</v>
       </c>
       <c r="B171" t="s">
-        <v>34</v>
+        <v>81</v>
+      </c>
+      <c r="C171">
+        <v>185</v>
       </c>
       <c r="D171" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E171" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="F171">
         <v>2007</v>
@@ -9469,13 +9779,16 @@
         <v>16</v>
       </c>
       <c r="B172" t="s">
-        <v>35</v>
+        <v>82</v>
+      </c>
+      <c r="C172">
+        <v>186</v>
       </c>
       <c r="D172" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E172" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F172">
         <v>2007</v>
@@ -9510,13 +9823,16 @@
         <v>17</v>
       </c>
       <c r="B173" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>129</v>
       </c>
       <c r="D173" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E173" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="F173">
         <v>2007</v>
@@ -9560,13 +9876,16 @@
         <v>18</v>
       </c>
       <c r="B174" t="s">
-        <v>7</v>
+        <v>54</v>
+      </c>
+      <c r="C174">
+        <v>168</v>
       </c>
       <c r="D174" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E174" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F174">
         <v>2007</v>
@@ -9607,13 +9926,16 @@
         <v>19</v>
       </c>
       <c r="B175" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="C175">
+        <v>161</v>
       </c>
       <c r="D175" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E175" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="F175">
         <v>2007</v>
@@ -9657,13 +9979,16 @@
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>36</v>
+        <v>83</v>
+      </c>
+      <c r="C176">
+        <v>187</v>
       </c>
       <c r="D176" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E176" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="F176">
         <v>2007</v>
@@ -9704,13 +10029,16 @@
         <v>21</v>
       </c>
       <c r="B177" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="C177">
+        <v>162</v>
       </c>
       <c r="D177" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E177" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="F177">
         <v>2007</v>
@@ -9748,13 +10076,16 @@
         <v>22</v>
       </c>
       <c r="B178" t="s">
-        <v>86</v>
+        <v>133</v>
+      </c>
+      <c r="C178">
+        <v>118</v>
       </c>
       <c r="D178" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E178" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="F178">
         <v>2007</v>
@@ -9792,13 +10123,16 @@
         <v>23</v>
       </c>
       <c r="B179" t="s">
-        <v>131</v>
+        <v>26</v>
+      </c>
+      <c r="C179">
+        <v>147</v>
       </c>
       <c r="D179" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E179" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="F179">
         <v>2007</v>
@@ -9833,13 +10167,16 @@
         <v>24</v>
       </c>
       <c r="B180" t="s">
-        <v>14</v>
+        <v>61</v>
+      </c>
+      <c r="C180">
+        <v>188</v>
       </c>
       <c r="D180" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E180" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="F180">
         <v>2007</v>
@@ -9883,13 +10220,16 @@
         <v>25</v>
       </c>
       <c r="B181" t="s">
-        <v>37</v>
+        <v>84</v>
+      </c>
+      <c r="C181">
+        <v>189</v>
       </c>
       <c r="D181" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E181" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="F181">
         <v>2007</v>
@@ -9933,13 +10273,16 @@
         <v>26</v>
       </c>
       <c r="B182" t="s">
-        <v>21</v>
+        <v>68</v>
+      </c>
+      <c r="C182">
+        <v>174</v>
       </c>
       <c r="D182" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E182" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="F182">
         <v>2007</v>
@@ -9977,13 +10320,16 @@
         <v>27</v>
       </c>
       <c r="B183" t="s">
-        <v>16</v>
+        <v>63</v>
+      </c>
+      <c r="C183">
+        <v>190</v>
       </c>
       <c r="D183" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E183" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="F183">
         <v>2007</v>
@@ -10024,13 +10370,16 @@
         <v>28</v>
       </c>
       <c r="B184" t="s">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="C184">
+        <v>191</v>
       </c>
       <c r="D184" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E184" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="F184">
         <v>2007</v>
@@ -10074,13 +10423,16 @@
         <v>29</v>
       </c>
       <c r="B185" t="s">
-        <v>38</v>
+        <v>85</v>
+      </c>
+      <c r="C185">
+        <v>192</v>
       </c>
       <c r="D185" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E185" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="F185">
         <v>2007</v>
@@ -10124,13 +10476,16 @@
         <v>30</v>
       </c>
       <c r="B186" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="C186">
+        <v>170</v>
       </c>
       <c r="D186" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E186" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F186">
         <v>2007</v>
@@ -10167,10 +10522,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>